<commit_message>
Managed employees scores against kpi's and sub kpi's. Handled Student module. Handled class held report and others minor changes in different controllers and models.
</commit_message>
<xml_diff>
--- a/Biit Employee Performance Apraisal API/CHR_Excel_Sheet/Book1.xlsx
+++ b/Biit Employee Performance Apraisal API/CHR_Excel_Sheet/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Course</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LateIn</t>
-  </si>
-  <si>
     <t>Left Early</t>
   </si>
   <si>
@@ -63,6 +60,12 @@
   </si>
   <si>
     <t>Held on time</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Late in</t>
   </si>
 </sst>
 </file>
@@ -118,17 +121,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H19" totalsRowShown="0">
-  <autoFilter ref="A1:H19"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I19" totalsRowShown="0">
+  <autoFilter ref="A1:I19"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Course"/>
     <tableColumn id="2" name="Teacher"/>
     <tableColumn id="3" name="Discipline"/>
     <tableColumn id="4" name="Venue"/>
     <tableColumn id="5" name="Status"/>
-    <tableColumn id="6" name="LateIn"/>
-    <tableColumn id="7" name="Left Early"/>
-    <tableColumn id="8" name="Remarks"/>
+    <tableColumn id="6" name="Session"/>
+    <tableColumn id="7" name="Late in"/>
+    <tableColumn id="8" name="Left Early"/>
+    <tableColumn id="9" name="Remarks"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -397,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -408,12 +412,12 @@
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
     <col min="2" max="2" width="16.36328125" customWidth="1"/>
     <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
     <col min="7" max="7" width="10.453125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,30 +434,33 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>